<commit_message>
Crit bonus changed slightly
+1 damage when phys, special effect otherwise
</commit_message>
<xml_diff>
--- a/Rules/Balancing Sheet.xlsx
+++ b/Rules/Balancing Sheet.xlsx
@@ -1747,7 +1747,7 @@
   <dimension ref="B2:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="O3" s="3">
         <f t="shared" ref="O3:O8" si="2">IF($U$5 &gt; 0,  IF(H3="X",0,  IF(I3="X", ($U$5-P3)/6,$U$5/6)      ),         0)</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P3" s="6">
         <f t="shared" ref="P3:P8" si="3">C3*M3</f>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="Q3" s="6">
         <f t="shared" ref="Q3:Q8" si="4">P3*N3*IF(H3="X",1,(1-O3))</f>
-        <v>0.16666666666666669</v>
+        <v>0.25</v>
       </c>
       <c r="R3" s="5"/>
       <c r="S3" t="s">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="O4" s="3">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" si="3"/>
@@ -1902,7 +1902,7 @@
       </c>
       <c r="Q4" s="6">
         <f t="shared" si="4"/>
-        <v>0.33333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="R4" s="5"/>
       <c r="S4" t="s">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="O5" s="3">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="3"/>
@@ -1950,13 +1950,13 @@
       </c>
       <c r="Q5" s="6">
         <f t="shared" si="4"/>
-        <v>0.22222222222222224</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S5" t="s">
         <v>31</v>
       </c>
       <c r="U5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="O7" s="3">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="3"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="Q7" s="6">
         <f t="shared" si="4"/>
-        <v>0.22222222222222224</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="O8" s="3">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="3"/>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="Q8" s="6">
         <f t="shared" si="4"/>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="O10" s="7">
         <f t="shared" ref="O10:O18" si="6">IF($U$5 &gt; 0,  IF(H10="X",0,  IF(I10="X", ($U$5-P10)/6,$U$5/6)      ),         0)</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" ref="P10:P18" si="7">C10*M10</f>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="Q10" s="8">
         <f t="shared" ref="Q10:Q15" si="8">P10*N10*IF(H10="X",1,(1-O10))</f>
-        <v>0.33333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="U10" t="s">
         <v>15</v>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="O11" s="7">
         <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" si="7"/>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="Q11" s="8">
         <f t="shared" si="8"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S11" t="s">
         <v>68</v>
@@ -2189,11 +2189,11 @@
         <v>2</v>
       </c>
       <c r="W11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X11" s="11">
         <f>U5/6</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="O12" s="7">
         <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" si="7"/>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="Q12" s="8">
         <f t="shared" si="8"/>
-        <v>0.44444444444444448</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="O14" s="7">
         <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" si="7"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="Q14" s="8">
         <f t="shared" si="8"/>
-        <v>0.29629629629629634</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="U14" s="11">
         <f>U11/6</f>
@@ -2329,11 +2329,11 @@
       </c>
       <c r="V14" s="11">
         <f>W11/6</f>
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="W14" s="12">
         <f>V11*U14*V14*(1-X11)</f>
-        <v>0.74074074074074081</v>
+        <v>1.3888888888888891</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="O15" s="7">
         <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
+        <v>0</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" si="7"/>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="Q15" s="8">
         <f t="shared" si="8"/>
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="O16" s="7">
         <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" si="7"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="Q16" s="8">
         <f>P16*N16*IF(H16="X",1,(1-O16))</f>
-        <v>0.33333333333333337</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="O18" s="7">
         <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="7"/>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="Q18" s="8">
         <f>P18*N18*IF(H18="X",1,(1-O18))</f>
-        <v>0.22222222222222224</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="O20" s="7">
         <f t="shared" ref="O20:O23" si="10">IF($U$5 &gt; 0,  IF(H20="X",0,  IF(I20="X", ($U$5-P20)/6,$U$5/6)      ),         0)</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" ref="P20:P23" si="11">C20*M20</f>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="Q20" s="8">
         <f t="shared" ref="Q20:Q23" si="12">P20*N20*IF(H20="X",1,(1-O20))</f>
-        <v>0.66666666666666674</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="O21" s="7">
         <f t="shared" si="10"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="11"/>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="Q21" s="8">
         <f t="shared" si="12"/>
-        <v>0.55555555555555569</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="O22" s="7">
         <f>IF($U$5 &gt; 0,  IF(H22="X",0,  IF(I22="X", ($U$5-P22)/6,$U$5/6)      ),         0)</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P22" s="8">
         <f>C22*M22</f>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="Q22" s="8">
         <f>P22*N22*IF(H22="X",1,(1-O22))</f>
-        <v>0.29629629629629634</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="O23" s="7">
         <f t="shared" si="10"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="11"/>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="12"/>
-        <v>0.29629629629629634</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Balance Changes, beginning of Campaign Rules
</commit_message>
<xml_diff>
--- a/Rules/Balancing Sheet.xlsx
+++ b/Rules/Balancing Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Melee Weapons P" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="79">
   <si>
     <t>Weapon</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Chaos</t>
+  </si>
+  <si>
+    <t>Dagger/Claw</t>
   </si>
 </sst>
 </file>
@@ -443,41 +446,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -537,6 +507,39 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -788,8 +791,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B2:Q11" totalsRowShown="0">
-  <autoFilter ref="B2:Q11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B2:Q10" totalsRowShown="0">
+  <autoFilter ref="B2:Q10"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Weapon"/>
     <tableColumn id="2" name="A   " dataDxfId="14"/>
@@ -808,14 +811,14 @@
     <tableColumn id="12" name="     Damage %" dataDxfId="10" dataCellStyle="Percent">
       <calculatedColumnFormula>D3/6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="     Armor Red." dataDxfId="9" dataCellStyle="Percent">
-      <calculatedColumnFormula>IF($V$5 &gt; 0,  IF(I3="X",0,  IF(J3="X", ($V$5-P3)/6,$V$5/6)      ),         0)</calculatedColumnFormula>
+    <tableColumn id="20" name="     Armor Red." dataDxfId="1" dataCellStyle="Percent">
+      <calculatedColumnFormula>IF($V$6 &gt; 0,  IF(I3="X",0,(7-$V$6)/6),         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="     Hits Æ" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="18" name="     Hits Æ" dataDxfId="9" dataCellStyle="Percent">
       <calculatedColumnFormula>C3*M3/E3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="     Wounds Æ" dataDxfId="7" dataCellStyle="Percent">
-      <calculatedColumnFormula>P3*N3*IF(I3="X",1,(1-O3))</calculatedColumnFormula>
+    <tableColumn id="19" name="     Wounds Æ" dataDxfId="0" dataCellStyle="Percent">
+      <calculatedColumnFormula>P3*N3*(1-O3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -827,8 +830,8 @@
   <autoFilter ref="B2:Q27"/>
   <tableColumns count="16">
     <tableColumn id="1" name="Weapon"/>
-    <tableColumn id="2" name="A   " dataDxfId="6"/>
-    <tableColumn id="3" name="D    " dataDxfId="5"/>
+    <tableColumn id="2" name="A   " dataDxfId="8"/>
+    <tableColumn id="3" name="D    " dataDxfId="7"/>
     <tableColumn id="4" name="Damage  "/>
     <tableColumn id="5" name="Type"/>
     <tableColumn id="17" name="Notes"/>
@@ -837,19 +840,19 @@
     <tableColumn id="8" name="Template"/>
     <tableColumn id="9" name="Column1"/>
     <tableColumn id="10" name=" "/>
-    <tableColumn id="11" name="     Hit %" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="11" name="     Hit %" dataDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(J3="X",4/6,($T$3/6))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="     Damage %" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="12" name="     Damage %" dataDxfId="5" dataCellStyle="Percent">
       <calculatedColumnFormula>D3/6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="     Armor Red." dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="20" name="     Armor Red." dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>IF($U$5 &gt; 0,  IF(H3="X",    IF($U$5&lt;4,0,0.5),  IF(I3="X", ($U$5-P3)/6,$U$5/6)      ),         0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="     Hits Æ" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="18" name="     Hits Æ" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>C3*M3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="     Wounds Æ" dataDxfId="0" dataCellStyle="Percent">
+    <tableColumn id="19" name="     Wounds Æ" dataDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>P3*N3*IF(H3="X",1,(1-O3))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2704,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V12"/>
+  <dimension ref="B2:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,13 +2777,13 @@
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -2791,37 +2794,33 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M9" si="0">(7 - (4-($U$4-$V$4)))/6</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="M3:M10" si="0">(7 - (4-($U$5-$V$5)))/6</f>
+        <v>0.5</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N9" si="1">D3/6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O3" s="3">
-        <f t="shared" ref="O3" si="2">IF($V$5 &gt; 0,  IF(I3="X",0,  IF(J3="X", ($V$5-P3)/6,$V$5/6)      ),         0)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P3" s="6">
-        <f t="shared" ref="P3:P9" si="3">C3*M3/E3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Q3" s="6">
-        <f>P3*N3*(1-O3)</f>
-        <v>0.14814814814814817</v>
-      </c>
-      <c r="R3" s="5"/>
-      <c r="T3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3">
-        <v>3</v>
+        <f>D3/6</f>
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="7">
+        <f t="shared" ref="O3:O12" si="1">IF($V$6 &gt; 0,  IF(I3="X",0,(7-$V$6)/6),         0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P3" s="8">
+        <f>C3*M3/E3</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="8">
+        <f t="shared" ref="Q3:Q10" si="2">P3*N3*(1-O3)</f>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -2838,43 +2837,37 @@
       <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
       <c r="M4" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="N4" s="3">
+        <f t="shared" ref="N4:N10" si="3">D4/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O4" s="7">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" ref="O4:O9" si="4">IF($V$5 &gt; 0,  IF(I4="X",0,  IF(J4="X", ($V$5-P4)/6,$V$5/6)      ),         0)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P4" s="6">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="P4:P10" si="4">C4*M4/E4</f>
+        <v>0.5</v>
       </c>
       <c r="Q4" s="6">
-        <f t="shared" ref="Q4:Q9" si="5">P4*N4*IF(I4="X",1,(1-O4))</f>
-        <v>0.22222222222222221</v>
+        <f t="shared" si="2"/>
+        <v>0.27777777777777779</v>
       </c>
       <c r="R4" s="5"/>
       <c r="T4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U4">
         <v>3</v>
       </c>
-      <c r="V4">
-        <v>4</v>
-      </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -2886,133 +2879,142 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" t="s">
         <v>32</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="6">
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
-      </c>
-      <c r="N5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="4"/>
-        <v>0.27777777777777779</v>
-      </c>
-      <c r="P5" s="6">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Q5" s="6">
-        <f t="shared" si="5"/>
-        <v>0.16049382716049382</v>
       </c>
       <c r="R5" s="5"/>
       <c r="T5" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
       </c>
       <c r="V5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
         <v>32</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="N6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O6" s="7">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="O6" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P6" s="6">
         <f t="shared" si="4"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P6" s="6">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="Q6" s="6">
-        <f t="shared" si="5"/>
-        <v>0.22222222222222224</v>
+        <f t="shared" si="2"/>
+        <v>0.27777777777777779</v>
       </c>
       <c r="R6" s="5"/>
+      <c r="T6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
         <v>32</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="N7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="7">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="O7" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P7" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="6">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="6">
-        <f t="shared" si="5"/>
-        <v>0.27777777777777779</v>
+        <f t="shared" si="2"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="R7" s="5"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -3024,45 +3026,45 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="N8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O8" s="7">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
         <f t="shared" si="4"/>
-        <v>0.27777777777777779</v>
-      </c>
-      <c r="P8" s="6">
-        <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="Q8" s="6">
-        <f t="shared" si="5"/>
-        <v>0.20061728395061729</v>
+        <f t="shared" si="2"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="R8" s="5"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -3071,39 +3073,72 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="N9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="O9" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P9" s="6">
         <f t="shared" si="4"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="P9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" s="6">
+        <f t="shared" si="2"/>
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="3">
         <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Q9" s="6">
-        <f t="shared" si="5"/>
-        <v>0.11111111111111112</v>
-      </c>
-      <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P10" s="6">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="6">
+        <f t="shared" si="2"/>
+        <v>0.20833333333333334</v>
+      </c>
       <c r="R10" s="5"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
@@ -3112,7 +3147,7 @@
       <c r="E11" s="1"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="5"/>
@@ -3123,10 +3158,21 @@
       <c r="E12" s="1"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="O12" s="7"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3141,7 +3187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>

</xml_diff>